<commit_message>
Se corrigen los titulos de las columnas
</commit_message>
<xml_diff>
--- a/Nevasa/CompraSimultanea/20240822/20240822_nevasa_compras_simultaneas_results.xlsx
+++ b/Nevasa/CompraSimultanea/20240822/20240822_nevasa_compras_simultaneas_results.xlsx
@@ -440,22 +440,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>instrumento</t>
+          <t>nemotecnico</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>monto_contado</t>
+          <t>monto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>monto_compromiso</t>
+          <t>cantidad</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>diferencia_precio</t>
+          <t>precio</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>